<commit_message>
Updated report and powerpoint
</commit_message>
<xml_diff>
--- a/ csc533/Project 2 - Bayesian Networks/data for project 2.xlsx
+++ b/ csc533/Project 2 - Bayesian Networks/data for project 2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="15195" windowHeight="8700"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="24765" windowHeight="14415"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,9 +418,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -438,9 +435,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,39 +442,45 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -783,7 +783,7 @@
   <dimension ref="A1:AV30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -798,22 +798,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" s="2" customFormat="1" ht="21.75" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>24</v>
       </c>
       <c r="G1" s="6"/>
@@ -860,16 +860,16 @@
       <c r="AV1" s="6"/>
     </row>
     <row r="2" spans="1:48" s="3" customFormat="1" ht="16.5" thickTop="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -929,7 +929,7 @@
       <c r="E3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="24" t="s">
         <v>25</v>
       </c>
       <c r="G3" s="6"/>
@@ -976,23 +976,23 @@
       <c r="AV3" s="6"/>
     </row>
     <row r="4" spans="1:48" s="4" customFormat="1" ht="15.75">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="19">
         <f>12500000/304059724</f>
         <v>4.1110344492715514E-2</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="25" t="s">
         <v>26</v>
       </c>
       <c r="G4" s="6"/>
@@ -1039,14 +1039,14 @@
       <c r="AV4" s="6"/>
     </row>
     <row r="5" spans="1:48" s="4" customFormat="1" ht="15">
-      <c r="A5" s="23"/>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="32"/>
+      <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="31"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -1091,13 +1091,13 @@
       <c r="AV5" s="6"/>
     </row>
     <row r="6" spans="1:48" s="4" customFormat="1" ht="30">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="35" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <f>AVERAGE(85.9, 26.9)/100000</f>
         <v>5.6400000000000005E-4</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>31</v>
       </c>
       <c r="E6" s="8"/>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="24" t="s">
         <v>29</v>
       </c>
       <c r="G6" s="6"/>
@@ -1152,11 +1152,11 @@
       <c r="AV6" s="6"/>
     </row>
     <row r="7" spans="1:48" s="4" customFormat="1" ht="30">
-      <c r="A7" s="11"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <f>AVERAGE(305.7, 157)/100000</f>
         <v>2.3135E-3</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="24" t="s">
         <v>29</v>
       </c>
       <c r="G7" s="6"/>
@@ -1211,22 +1211,22 @@
       <c r="AV7" s="6"/>
     </row>
     <row r="8" spans="1:48" s="4" customFormat="1" ht="15.75">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="19">
         <v>4.4499999999999998E-2</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="26" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="6"/>
@@ -1273,21 +1273,21 @@
       <c r="AV8" s="6"/>
     </row>
     <row r="9" spans="1:48" s="4" customFormat="1" ht="15.75">
-      <c r="A9" s="23"/>
-      <c r="B9" s="20" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="19">
         <f>4.23*C8</f>
         <v>0.18823500000000001</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="26" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="6"/>
@@ -1334,13 +1334,13 @@
       <c r="AV9" s="6"/>
     </row>
     <row r="10" spans="1:48" s="4" customFormat="1" ht="45">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="35" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <f>AVERAGE(10,37)/100</f>
         <v>0.23499999999999999</v>
       </c>
@@ -1350,7 +1350,7 @@
       <c r="E10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="24" t="s">
         <v>40</v>
       </c>
       <c r="G10" s="6"/>
@@ -1397,7 +1397,7 @@
       <c r="AV10" s="6"/>
     </row>
     <row r="11" spans="1:48" s="4" customFormat="1" ht="15.75">
-      <c r="A11" s="11"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="8" t="s">
         <v>16</v>
       </c>
@@ -1410,7 +1410,7 @@
       <c r="E11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="27" t="s">
         <v>36</v>
       </c>
       <c r="G11" s="6"/>
@@ -1456,8 +1456,8 @@
       <c r="AU11" s="6"/>
       <c r="AV11" s="6"/>
     </row>
-    <row r="12" spans="1:48" s="4" customFormat="1" ht="15.75">
-      <c r="A12" s="11"/>
+    <row r="12" spans="1:48" s="4" customFormat="1" ht="30.75">
+      <c r="A12" s="35"/>
       <c r="B12" s="8" t="s">
         <v>17</v>
       </c>
@@ -1470,7 +1470,7 @@
       <c r="E12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="27" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="6"/>
@@ -1517,14 +1517,14 @@
       <c r="AV12" s="6"/>
     </row>
     <row r="13" spans="1:48" s="4" customFormat="1" ht="15">
-      <c r="A13" s="11"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="10"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="29"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -1568,23 +1568,23 @@
       <c r="AU13" s="6"/>
       <c r="AV13" s="6"/>
     </row>
-    <row r="14" spans="1:48" s="4" customFormat="1" ht="15.75">
-      <c r="A14" s="19" t="s">
+    <row r="14" spans="1:48" s="4" customFormat="1" ht="30.75">
+      <c r="A14" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="19">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="26" t="s">
         <v>50</v>
       </c>
       <c r="G14" s="6"/>
@@ -1630,21 +1630,21 @@
       <c r="AU14" s="6"/>
       <c r="AV14" s="6"/>
     </row>
-    <row r="15" spans="1:48" s="4" customFormat="1" ht="75.75">
-      <c r="A15" s="25"/>
-      <c r="B15" s="20" t="s">
+    <row r="15" spans="1:48" s="4" customFormat="1" ht="105.75">
+      <c r="A15" s="33"/>
+      <c r="B15" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="19">
         <v>0.432</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="28" t="s">
         <v>48</v>
       </c>
       <c r="G15" s="6"/>
@@ -1691,21 +1691,21 @@
       <c r="AV15" s="6"/>
     </row>
     <row r="16" spans="1:48" s="4" customFormat="1" ht="30.75">
-      <c r="A16" s="25"/>
-      <c r="B16" s="20" t="s">
+      <c r="A16" s="33"/>
+      <c r="B16" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="19">
         <f>AVERAGE(20,60)/100</f>
         <v>0.4</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="25" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="6"/>
@@ -1752,21 +1752,21 @@
       <c r="AV16" s="6"/>
     </row>
     <row r="17" spans="1:48" s="5" customFormat="1" ht="30.75">
-      <c r="A17" s="25"/>
-      <c r="B17" s="20" t="s">
+      <c r="A17" s="33"/>
+      <c r="B17" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="19">
         <f>AVERAGE(19.4, 22)/100</f>
         <v>0.20699999999999999</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="26" t="s">
         <v>50</v>
       </c>
       <c r="G17" s="6"/>
@@ -1813,14 +1813,14 @@
       <c r="AV17" s="6"/>
     </row>
     <row r="18" spans="1:48" s="2" customFormat="1" ht="15">
-      <c r="A18" s="25"/>
-      <c r="B18" s="20" t="s">
+      <c r="A18" s="33"/>
+      <c r="B18" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="34"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1865,14 +1865,14 @@
       <c r="AV18" s="6"/>
     </row>
     <row r="19" spans="1:48" s="2" customFormat="1" ht="15">
-      <c r="A19" s="25"/>
-      <c r="B19" s="20" t="s">
+      <c r="A19" s="33"/>
+      <c r="B19" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="34"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="29"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -1917,14 +1917,14 @@
       <c r="AV19" s="6"/>
     </row>
     <row r="20" spans="1:48" s="2" customFormat="1" ht="15">
-      <c r="A20" s="25"/>
-      <c r="B20" s="20" t="s">
+      <c r="A20" s="33"/>
+      <c r="B20" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="34"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="29"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -1969,14 +1969,14 @@
       <c r="AV20" s="6"/>
     </row>
     <row r="21" spans="1:48" s="2" customFormat="1" ht="15">
-      <c r="A21" s="27"/>
-      <c r="B21" s="20" t="s">
+      <c r="A21" s="34"/>
+      <c r="B21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="34"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="29"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -2021,69 +2021,69 @@
       <c r="AV21" s="6"/>
     </row>
     <row r="22" spans="1:48">
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
-      <c r="X22" s="35"/>
-      <c r="Y22" s="35"/>
-      <c r="Z22" s="35"/>
-      <c r="AA22" s="35"/>
-      <c r="AB22" s="35"/>
-      <c r="AC22" s="35"/>
-      <c r="AD22" s="35"/>
-      <c r="AE22" s="35"/>
-      <c r="AF22" s="35"/>
-      <c r="AG22" s="35"/>
-      <c r="AH22" s="35"/>
-      <c r="AI22" s="35"/>
-      <c r="AJ22" s="35"/>
-      <c r="AK22" s="35"/>
-      <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
-      <c r="AN22" s="35"/>
-      <c r="AO22" s="35"/>
-      <c r="AP22" s="35"/>
-      <c r="AQ22" s="35"/>
-      <c r="AR22" s="35"/>
-      <c r="AS22" s="35"/>
-      <c r="AT22" s="35"/>
-      <c r="AU22" s="35"/>
-      <c r="AV22" s="35"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
+      <c r="U22" s="30"/>
+      <c r="V22" s="30"/>
+      <c r="W22" s="30"/>
+      <c r="X22" s="30"/>
+      <c r="Y22" s="30"/>
+      <c r="Z22" s="30"/>
+      <c r="AA22" s="30"/>
+      <c r="AB22" s="30"/>
+      <c r="AC22" s="30"/>
+      <c r="AD22" s="30"/>
+      <c r="AE22" s="30"/>
+      <c r="AF22" s="30"/>
+      <c r="AG22" s="30"/>
+      <c r="AH22" s="30"/>
+      <c r="AI22" s="30"/>
+      <c r="AJ22" s="30"/>
+      <c r="AK22" s="30"/>
+      <c r="AL22" s="30"/>
+      <c r="AM22" s="30"/>
+      <c r="AN22" s="30"/>
+      <c r="AO22" s="30"/>
+      <c r="AP22" s="30"/>
+      <c r="AQ22" s="30"/>
+      <c r="AR22" s="30"/>
+      <c r="AS22" s="30"/>
+      <c r="AT22" s="30"/>
+      <c r="AU22" s="30"/>
+      <c r="AV22" s="30"/>
     </row>
     <row r="23" spans="1:48">
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="35"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
-      <c r="X23" s="35"/>
-      <c r="Y23" s="35"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="30"/>
+      <c r="V23" s="30"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="30"/>
     </row>
     <row r="30" spans="1:48">
       <c r="E30" s="1"/>
@@ -2101,7 +2101,7 @@
     <hyperlink ref="F4" r:id="rId1"/>
     <hyperlink ref="F12" r:id="rId2"/>
     <hyperlink ref="F11" r:id="rId3"/>
-    <hyperlink ref="F15"/>
+    <hyperlink ref="F15" display="http://books.google.com/books?id=iWnwrHy3uF0C&amp;pg=PA316&amp;lpg=PA316&amp;dq=frequency+dyspnea+tuberculosis&amp;source=bl&amp;ots=44xqrQ96Vg&amp;sig=9tR9Lah_Lj_IEEwzrqA8yLayvzQ&amp;hl=en&amp;ei=iCv6SrGoHtL-nQfa7Oz0DA&amp;sa=X&amp;oi=book_result&amp;ct=result&amp;resnum=9&amp;ved=0CDMQ6AEwCA#v=onepage&amp;q="/>
     <hyperlink ref="F16" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More Updating on Report and PowerPoint
</commit_message>
<xml_diff>
--- a/ csc533/Project 2 - Bayesian Networks/data for project 2.xlsx
+++ b/ csc533/Project 2 - Bayesian Networks/data for project 2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>Trait</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>chronic bronchitis; up to 94% at end of life for COPD</t>
+  </si>
+  <si>
+    <t>REASONABLE GUESS</t>
   </si>
 </sst>
 </file>
@@ -240,14 +243,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <i/>
-      <u/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +272,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,16 +427,11 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -442,7 +446,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -452,16 +455,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -480,6 +474,23 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="5" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="5" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -783,7 +794,7 @@
   <dimension ref="A1:AV30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -798,22 +809,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" s="2" customFormat="1" ht="21.75" thickBot="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>24</v>
       </c>
       <c r="G1" s="6"/>
@@ -860,16 +871,20 @@
       <c r="AV1" s="6"/>
     </row>
     <row r="2" spans="1:48" s="3" customFormat="1" ht="16.5" thickTop="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="23"/>
+      <c r="C2" s="34">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -929,7 +944,7 @@
       <c r="E3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="30" t="s">
         <v>25</v>
       </c>
       <c r="G3" s="6"/>
@@ -976,23 +991,23 @@
       <c r="AV3" s="6"/>
     </row>
     <row r="4" spans="1:48" s="4" customFormat="1" ht="15.75">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="16">
         <f>12500000/304059724</f>
         <v>4.1110344492715514E-2</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="29" t="s">
         <v>26</v>
       </c>
       <c r="G4" s="6"/>
@@ -1039,14 +1054,18 @@
       <c r="AV4" s="6"/>
     </row>
     <row r="5" spans="1:48" s="4" customFormat="1" ht="15">
-      <c r="A5" s="32"/>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="26"/>
+      <c r="C5" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -1090,14 +1109,14 @@
       <c r="AU5" s="6"/>
       <c r="AV5" s="6"/>
     </row>
-    <row r="6" spans="1:48" s="4" customFormat="1" ht="30">
-      <c r="A6" s="35" t="s">
+    <row r="6" spans="1:48" s="4" customFormat="1" ht="30.75">
+      <c r="A6" s="28" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <f>AVERAGE(85.9, 26.9)/100000</f>
         <v>5.6400000000000005E-4</v>
       </c>
@@ -1105,7 +1124,7 @@
         <v>31</v>
       </c>
       <c r="E6" s="8"/>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="30" t="s">
         <v>29</v>
       </c>
       <c r="G6" s="6"/>
@@ -1151,12 +1170,12 @@
       <c r="AU6" s="6"/>
       <c r="AV6" s="6"/>
     </row>
-    <row r="7" spans="1:48" s="4" customFormat="1" ht="30">
-      <c r="A7" s="35"/>
+    <row r="7" spans="1:48" s="4" customFormat="1" ht="30.75">
+      <c r="A7" s="28"/>
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <f>AVERAGE(305.7, 157)/100000</f>
         <v>2.3135E-3</v>
       </c>
@@ -1164,7 +1183,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="30" t="s">
         <v>29</v>
       </c>
       <c r="G7" s="6"/>
@@ -1211,22 +1230,22 @@
       <c r="AV7" s="6"/>
     </row>
     <row r="8" spans="1:48" s="4" customFormat="1" ht="15.75">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="16">
         <v>4.4499999999999998E-2</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="29" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="6"/>
@@ -1273,21 +1292,21 @@
       <c r="AV8" s="6"/>
     </row>
     <row r="9" spans="1:48" s="4" customFormat="1" ht="15.75">
-      <c r="A9" s="32"/>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="16">
         <f>4.23*C8</f>
         <v>0.18823500000000001</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="6"/>
@@ -1333,14 +1352,14 @@
       <c r="AU9" s="6"/>
       <c r="AV9" s="6"/>
     </row>
-    <row r="10" spans="1:48" s="4" customFormat="1" ht="45">
-      <c r="A10" s="35" t="s">
+    <row r="10" spans="1:48" s="4" customFormat="1" ht="45.75">
+      <c r="A10" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <f>AVERAGE(10,37)/100</f>
         <v>0.23499999999999999</v>
       </c>
@@ -1350,7 +1369,7 @@
       <c r="E10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="30" t="s">
         <v>40</v>
       </c>
       <c r="G10" s="6"/>
@@ -1397,7 +1416,7 @@
       <c r="AV10" s="6"/>
     </row>
     <row r="11" spans="1:48" s="4" customFormat="1" ht="15.75">
-      <c r="A11" s="35"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="8" t="s">
         <v>16</v>
       </c>
@@ -1410,7 +1429,7 @@
       <c r="E11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="30" t="s">
         <v>36</v>
       </c>
       <c r="G11" s="6"/>
@@ -1456,8 +1475,8 @@
       <c r="AU11" s="6"/>
       <c r="AV11" s="6"/>
     </row>
-    <row r="12" spans="1:48" s="4" customFormat="1" ht="30.75">
-      <c r="A12" s="35"/>
+    <row r="12" spans="1:48" s="4" customFormat="1" ht="15.75">
+      <c r="A12" s="28"/>
       <c r="B12" s="8" t="s">
         <v>17</v>
       </c>
@@ -1470,7 +1489,7 @@
       <c r="E12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="30" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="6"/>
@@ -1517,14 +1536,18 @@
       <c r="AV12" s="6"/>
     </row>
     <row r="13" spans="1:48" s="4" customFormat="1" ht="15">
-      <c r="A13" s="35"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10"/>
+      <c r="C13" s="32">
+        <v>0.95</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>56</v>
+      </c>
       <c r="E13" s="8"/>
-      <c r="F13" s="24"/>
+      <c r="F13" s="20"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -1568,23 +1591,23 @@
       <c r="AU13" s="6"/>
       <c r="AV13" s="6"/>
     </row>
-    <row r="14" spans="1:48" s="4" customFormat="1" ht="30.75">
-      <c r="A14" s="31" t="s">
+    <row r="14" spans="1:48" s="4" customFormat="1" ht="15.75">
+      <c r="A14" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="16">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="29" t="s">
         <v>50</v>
       </c>
       <c r="G14" s="6"/>
@@ -1630,21 +1653,21 @@
       <c r="AU14" s="6"/>
       <c r="AV14" s="6"/>
     </row>
-    <row r="15" spans="1:48" s="4" customFormat="1" ht="105.75">
-      <c r="A15" s="33"/>
-      <c r="B15" s="18" t="s">
+    <row r="15" spans="1:48" s="4" customFormat="1" ht="64.5">
+      <c r="A15" s="26"/>
+      <c r="B15" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="16">
         <v>0.432</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="31" t="s">
         <v>48</v>
       </c>
       <c r="G15" s="6"/>
@@ -1691,21 +1714,21 @@
       <c r="AV15" s="6"/>
     </row>
     <row r="16" spans="1:48" s="4" customFormat="1" ht="30.75">
-      <c r="A16" s="33"/>
-      <c r="B16" s="18" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="16">
         <f>AVERAGE(20,60)/100</f>
         <v>0.4</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="29" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="6"/>
@@ -1752,21 +1775,21 @@
       <c r="AV16" s="6"/>
     </row>
     <row r="17" spans="1:48" s="5" customFormat="1" ht="30.75">
-      <c r="A17" s="33"/>
-      <c r="B17" s="18" t="s">
+      <c r="A17" s="26"/>
+      <c r="B17" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="16">
         <f>AVERAGE(19.4, 22)/100</f>
         <v>0.20699999999999999</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="29" t="s">
         <v>50</v>
       </c>
       <c r="G17" s="6"/>
@@ -1813,14 +1836,18 @@
       <c r="AV17" s="6"/>
     </row>
     <row r="18" spans="1:48" s="2" customFormat="1" ht="15">
-      <c r="A18" s="33"/>
-      <c r="B18" s="18" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="29"/>
+      <c r="C18" s="32">
+        <v>0.6</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="22"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1865,14 +1892,18 @@
       <c r="AV18" s="6"/>
     </row>
     <row r="19" spans="1:48" s="2" customFormat="1" ht="15">
-      <c r="A19" s="33"/>
-      <c r="B19" s="18" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="29"/>
+      <c r="C19" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="22"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -1917,14 +1948,18 @@
       <c r="AV19" s="6"/>
     </row>
     <row r="20" spans="1:48" s="2" customFormat="1" ht="15">
-      <c r="A20" s="33"/>
-      <c r="B20" s="18" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="29"/>
+      <c r="C20" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="22"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -1969,14 +2004,18 @@
       <c r="AV20" s="6"/>
     </row>
     <row r="21" spans="1:48" s="2" customFormat="1" ht="15">
-      <c r="A21" s="34"/>
-      <c r="B21" s="18" t="s">
+      <c r="A21" s="27"/>
+      <c r="B21" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="29"/>
+      <c r="C21" s="32">
+        <v>0.75</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="22"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -2021,69 +2060,69 @@
       <c r="AV21" s="6"/>
     </row>
     <row r="22" spans="1:48">
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
-      <c r="S22" s="30"/>
-      <c r="T22" s="30"/>
-      <c r="U22" s="30"/>
-      <c r="V22" s="30"/>
-      <c r="W22" s="30"/>
-      <c r="X22" s="30"/>
-      <c r="Y22" s="30"/>
-      <c r="Z22" s="30"/>
-      <c r="AA22" s="30"/>
-      <c r="AB22" s="30"/>
-      <c r="AC22" s="30"/>
-      <c r="AD22" s="30"/>
-      <c r="AE22" s="30"/>
-      <c r="AF22" s="30"/>
-      <c r="AG22" s="30"/>
-      <c r="AH22" s="30"/>
-      <c r="AI22" s="30"/>
-      <c r="AJ22" s="30"/>
-      <c r="AK22" s="30"/>
-      <c r="AL22" s="30"/>
-      <c r="AM22" s="30"/>
-      <c r="AN22" s="30"/>
-      <c r="AO22" s="30"/>
-      <c r="AP22" s="30"/>
-      <c r="AQ22" s="30"/>
-      <c r="AR22" s="30"/>
-      <c r="AS22" s="30"/>
-      <c r="AT22" s="30"/>
-      <c r="AU22" s="30"/>
-      <c r="AV22" s="30"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
+      <c r="W22" s="23"/>
+      <c r="X22" s="23"/>
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="23"/>
+      <c r="AA22" s="23"/>
+      <c r="AB22" s="23"/>
+      <c r="AC22" s="23"/>
+      <c r="AD22" s="23"/>
+      <c r="AE22" s="23"/>
+      <c r="AF22" s="23"/>
+      <c r="AG22" s="23"/>
+      <c r="AH22" s="23"/>
+      <c r="AI22" s="23"/>
+      <c r="AJ22" s="23"/>
+      <c r="AK22" s="23"/>
+      <c r="AL22" s="23"/>
+      <c r="AM22" s="23"/>
+      <c r="AN22" s="23"/>
+      <c r="AO22" s="23"/>
+      <c r="AP22" s="23"/>
+      <c r="AQ22" s="23"/>
+      <c r="AR22" s="23"/>
+      <c r="AS22" s="23"/>
+      <c r="AT22" s="23"/>
+      <c r="AU22" s="23"/>
+      <c r="AV22" s="23"/>
     </row>
     <row r="23" spans="1:48">
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="30"/>
-      <c r="T23" s="30"/>
-      <c r="U23" s="30"/>
-      <c r="V23" s="30"/>
-      <c r="W23" s="30"/>
-      <c r="X23" s="30"/>
-      <c r="Y23" s="30"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="23"/>
+      <c r="X23" s="23"/>
+      <c r="Y23" s="23"/>
     </row>
     <row r="30" spans="1:48">
       <c r="E30" s="1"/>
@@ -2101,11 +2140,19 @@
     <hyperlink ref="F4" r:id="rId1"/>
     <hyperlink ref="F12" r:id="rId2"/>
     <hyperlink ref="F11" r:id="rId3"/>
-    <hyperlink ref="F15" display="http://books.google.com/books?id=iWnwrHy3uF0C&amp;pg=PA316&amp;lpg=PA316&amp;dq=frequency+dyspnea+tuberculosis&amp;source=bl&amp;ots=44xqrQ96Vg&amp;sig=9tR9Lah_Lj_IEEwzrqA8yLayvzQ&amp;hl=en&amp;ei=iCv6SrGoHtL-nQfa7Oz0DA&amp;sa=X&amp;oi=book_result&amp;ct=result&amp;resnum=9&amp;ved=0CDMQ6AEwCA#v=onepage&amp;q="/>
+    <hyperlink ref="F15"/>
     <hyperlink ref="F16" r:id="rId4"/>
+    <hyperlink ref="F3" r:id="rId5"/>
+    <hyperlink ref="F6" r:id="rId6"/>
+    <hyperlink ref="F7" r:id="rId7"/>
+    <hyperlink ref="F8" r:id="rId8"/>
+    <hyperlink ref="F9" r:id="rId9"/>
+    <hyperlink ref="F14" r:id="rId10"/>
+    <hyperlink ref="F17" r:id="rId11"/>
+    <hyperlink ref="F10" r:id="rId12" display="http://www3.interscience.wiley.com/cgi-bin/fulltext/76501988/HTMLSTART"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="74" orientation="landscape" horizontalDpi="4294967293" r:id="rId5"/>
+  <pageSetup scale="74" orientation="landscape" horizontalDpi="4294967293" r:id="rId13"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>